<commit_message>
automation done git add .! :)
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21697\OneDrive\Documents\Visual Studio\HTML\Angular\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B36D5BF-1E27-4BE5-8AA9-A8CDE47558BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F2C12-23C8-42A2-9F39-D45A2EC0298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DD29A0ED-4022-4E63-8102-C98A077501F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD29A0ED-4022-4E63-8102-C98A077501F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869940BA-D568-45DD-87F0-4FCDCFF6B845}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +561,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>

</xml_diff>